<commit_message>
Minor fixes to Generate ID script
</commit_message>
<xml_diff>
--- a/Supporting Scripts/Static_Variables/Words.xlsx
+++ b/Supporting Scripts/Static_Variables/Words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kokal\Desktop\Work\Github Repos\Mine\Animate-Inanimate\Supporting Scripts\Static_Variables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EMU - Behavior\Documents\MATLAB\Behavioral Tasks\BH\Animate-Inanimate\Supporting Scripts\Static_Variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC0547-E580-4936-A63C-9D903F480638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FE208E-6273-49E2-B02D-148846EA817F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{03393A37-0A1C-43C2-818B-D3E00CD9CCC5}"/>
+    <workbookView xWindow="6285" yWindow="2385" windowWidth="19095" windowHeight="11385" xr2:uid="{03393A37-0A1C-43C2-818B-D3E00CD9CCC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D9B854-3E56-409D-B5EC-5DF461F0696E}">
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="E134" sqref="D1:E134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>